<commit_message>
Updating filtered feeds from workflow
</commit_message>
<xml_diff>
--- a/filtered_feeds.xlsx
+++ b/filtered_feeds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>link</t>
   </si>
@@ -22,6 +22,9 @@
     <t>keywords</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>http://www.fda.gov/drugs/resources-information-approved-drugs/fda-disco-burst-edition-fda-approvals-augtyro-repotrectinib-ntrk-gene-fusion-positive-solid-tumors</t>
   </si>
   <si>
@@ -65,6 +68,33 @@
   </si>
   <si>
     <t>ctDNA</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approvals of Augtyro (repotrectinib) for NTRK gene fusion-positive solid tumors and Krazati (adagrasib) for KRAS G12C-mutated colorectal cancer</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approvals of Tecentriq (atezolizumab) for unresectable or metastatic alveolar soft part sarcoma, and Krazati (adagrasib) for KRAS G12C-mutated locally advanced or metastatic non-small cell lung cancer</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approval of Vijoice (alpelisib) for adult and pediatric patients two years of age and older with severe manifestations of PIK3CA-related overgrowth spectrum who require systemic therapy</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approvals of Verzenio (abemaciclib) for adjuvant treatment of adult patients with hormone receptor-positive, human epidermal growth factor receptor 2-negative, node-positive, early breast cancer, &amp; Keytruda (pembrolizumab) for persistent, recurrent or metastatic cervical cancer whose tumors express PD-L1 (CPS ≥1)</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approvals of Lumakras (sotorasib) for patients with KRAS G12C  mutated locally advanced or metastatic non-small cell lung cancer, and Truseltiq (infigratinib) for unresectable locally advanced or metastatic cholangiocarcinoma with a fibroblast growth factor receptor 2 fusion or other rearrangement</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: FDA approvals of Trodelvy (sacituzumab govitecan) for locally advanced/metastatic urothelial cancer who received platinum-containing chemotherapy &amp; either PD-1/PD-L1 inhibitor and Opdivo (nivolumab) in combination with chemotherapy for metastatic gastric cancer and esophageal adenocarcinoma</t>
+  </si>
+  <si>
+    <t>FDA D.I.S.C.O. Burst Edition: Libtayo (cemiplimab-rwlc) for first-line treatment of patients with advanced NSCLC (locally advanced who are not candidates for surgical resection or definitive chemoradiation or metastatic) whose tumors have high PD-L1 expression with no eGFR, anaplastic lymphoma kinase or receptor tyrosine kinase aberrations</t>
+  </si>
+  <si>
+    <t>Lumea to Incorporate Myriad Genetics Cancer Tests Into Digital Pathology Platform</t>
+  </si>
+  <si>
+    <t>Natera MRD Study Results Demonstrate Potential to Ressurect Failed Adjuvant Drugs</t>
   </si>
 </sst>
 </file>
@@ -435,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,110 +473,150 @@
   <cols>
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
+      <c r="C13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>